<commit_message>
Adds attribution to "broken" version of prog-mod dataset.
</commit_message>
<xml_diff>
--- a/files/prog-mod/oceania-uk.xlsx
+++ b/files/prog-mod/oceania-uk.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>continent</t>
   </si>
@@ -36,9 +36,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>GDP per capita, life expectancy, and population size for Australia and New Zealand</t>
-  </si>
-  <si>
     <t>5-year period</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>Need to check Australian polit. situation in mid-1990s.</t>
+  </si>
+  <si>
+    <t>GDP per capita, life expectancy, and population size for Australia and the United Kingdom</t>
+  </si>
+  <si>
+    <t>(taken from Gapminder dataset, http://gapminder.org/data)</t>
   </si>
 </sst>
 </file>
@@ -125,12 +128,12 @@
       <b/>
       <u/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +144,12 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -172,11 +181,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -184,6 +192,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -469,7 +479,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -492,8 +502,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
+      <c r="A1" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -502,448 +512,419 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1952</v>
-      </c>
-      <c r="C4">
-        <v>8691212</v>
-      </c>
-      <c r="D4">
-        <v>69.12</v>
-      </c>
-      <c r="E4">
-        <v>10039.59564</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>1952</v>
-      </c>
-      <c r="K4">
-        <v>50430000</v>
-      </c>
-      <c r="L4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4">
-        <v>69.180000000000007</v>
-      </c>
-      <c r="N4">
-        <v>9979.5084869999991</v>
-      </c>
-      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1957</v>
+        <v>1952</v>
       </c>
       <c r="C5">
-        <v>9712569</v>
+        <v>8691212</v>
       </c>
       <c r="D5">
-        <v>70.33</v>
+        <v>69.12</v>
       </c>
       <c r="E5">
-        <v>10949.649590000001</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>10039.59564</v>
+      </c>
+      <c r="G5" s="3"/>
       <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>1952</v>
+      </c>
+      <c r="K5">
+        <v>50430000</v>
+      </c>
+      <c r="L5" t="s">
         <v>12</v>
       </c>
-      <c r="J5">
-        <v>1957</v>
-      </c>
-      <c r="K5">
-        <v>51430000</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
       <c r="M5">
-        <v>70.42</v>
+        <v>69.180000000000007</v>
       </c>
       <c r="N5">
-        <v>11283.177949999999</v>
-      </c>
-      <c r="P5" s="4"/>
+        <v>9979.5084869999991</v>
+      </c>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1962</v>
+        <v>1957</v>
       </c>
       <c r="C6">
-        <v>10794968</v>
+        <v>9712569</v>
       </c>
       <c r="D6">
-        <v>70.930000000000007</v>
+        <v>70.33</v>
       </c>
       <c r="E6">
-        <v>12217.226860000001</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>10949.649590000001</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6">
-        <v>1962</v>
+        <v>1957</v>
       </c>
       <c r="K6">
-        <v>53292000</v>
+        <v>51430000</v>
       </c>
       <c r="L6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M6">
-        <v>70.760000000000005</v>
+        <v>70.42</v>
       </c>
       <c r="N6">
-        <v>12477.17707</v>
-      </c>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="30">
+        <v>11283.177949999999</v>
+      </c>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>1967</v>
+        <v>1962</v>
       </c>
       <c r="C7">
-        <v>11872264</v>
+        <v>10794968</v>
       </c>
       <c r="D7">
-        <v>71.099999999999994</v>
+        <v>70.930000000000007</v>
       </c>
       <c r="E7">
-        <v>14526.12465</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>12217.226860000001</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7">
-        <v>1967</v>
+        <v>1962</v>
       </c>
       <c r="K7">
-        <v>54959000</v>
+        <v>53292000</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M7">
-        <v>71.36</v>
+        <v>70.760000000000005</v>
       </c>
       <c r="N7">
-        <v>14142.85089</v>
-      </c>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16">
+        <v>12477.17707</v>
+      </c>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" ht="30">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>1972</v>
+        <v>1967</v>
       </c>
       <c r="C8">
-        <v>13177000</v>
+        <v>11872264</v>
       </c>
       <c r="D8">
-        <v>71.930000000000007</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="E8">
-        <v>16788.62948</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>14526.12465</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8">
-        <v>1972</v>
+        <v>1967</v>
       </c>
       <c r="K8">
-        <v>56079000</v>
+        <v>54959000</v>
       </c>
       <c r="L8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M8">
-        <v>72.010000000000005</v>
+        <v>71.36</v>
       </c>
       <c r="N8">
-        <v>15895.116410000001</v>
-      </c>
-      <c r="P8" s="4"/>
+        <v>14142.85089</v>
+      </c>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>1977</v>
+        <v>1972</v>
       </c>
       <c r="C9">
-        <v>14074100</v>
+        <v>13177000</v>
       </c>
       <c r="D9">
-        <v>73.489999999999995</v>
+        <v>71.930000000000007</v>
       </c>
       <c r="E9">
-        <v>18334.197510000002</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>16788.62948</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9">
         <v>1972</v>
       </c>
       <c r="K9">
-        <v>56179000</v>
+        <v>56079000</v>
       </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M9">
-        <v>72.760000000000005</v>
+        <v>72.010000000000005</v>
       </c>
       <c r="N9">
-        <v>17428.748459999999</v>
-      </c>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="30">
+        <v>15895.116410000001</v>
+      </c>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>1982</v>
+        <v>1977</v>
       </c>
       <c r="C10">
-        <v>15184200</v>
+        <v>14074100</v>
       </c>
       <c r="D10">
-        <v>74.739999999999995</v>
+        <v>73.489999999999995</v>
       </c>
       <c r="E10">
-        <v>19477.009279999998</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>18334.197510000002</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10">
-        <v>1982</v>
+        <v>1972</v>
       </c>
       <c r="K10">
-        <v>56339704</v>
+        <v>56179000</v>
       </c>
       <c r="L10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M10">
-        <v>74.040000000000006</v>
-      </c>
-      <c r="N10" t="s">
-        <v>4</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>72.760000000000005</v>
+      </c>
+      <c r="N10">
+        <v>17428.748459999999</v>
+      </c>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" ht="30">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>1987</v>
+        <v>1982</v>
       </c>
       <c r="C11">
-        <v>16257249</v>
+        <v>15184200</v>
       </c>
       <c r="D11">
-        <v>76.319999999999993</v>
+        <v>74.739999999999995</v>
       </c>
       <c r="E11">
-        <v>21888.889029999998</v>
-      </c>
-      <c r="G11" s="4"/>
+        <v>19477.009279999998</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11">
-        <v>1987</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
+        <v>1982</v>
+      </c>
+      <c r="K11">
+        <v>56339704</v>
       </c>
       <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11">
+        <v>74.040000000000006</v>
+      </c>
+      <c r="N11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M11">
-        <v>75.007000000000005</v>
-      </c>
-      <c r="N11">
-        <v>21664.787670000002</v>
-      </c>
-      <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="C12">
-        <v>17481977</v>
+        <v>16257249</v>
       </c>
       <c r="D12">
-        <v>77.56</v>
+        <v>76.319999999999993</v>
       </c>
       <c r="E12">
-        <v>23424.76683</v>
-      </c>
+        <v>21888.889029999998</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12">
-        <v>1992</v>
-      </c>
-      <c r="K12">
-        <v>57866349</v>
+        <v>1987</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M12">
-        <v>76.42</v>
+        <v>75.007000000000005</v>
       </c>
       <c r="N12">
-        <v>22705.092540000001</v>
-      </c>
-      <c r="P12" s="4"/>
+        <v>21664.787670000002</v>
+      </c>
+      <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>1997</v>
+        <v>1992</v>
       </c>
       <c r="C13">
-        <v>18565243</v>
+        <v>17481977</v>
       </c>
       <c r="D13">
-        <v>78.83</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>77.56</v>
+      </c>
+      <c r="E13">
+        <v>23424.76683</v>
+      </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13">
-        <v>1997</v>
+        <v>1992</v>
       </c>
       <c r="K13">
-        <v>58808266</v>
+        <v>57866349</v>
       </c>
       <c r="L13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M13">
-        <v>77.218000000000004</v>
+        <v>76.42</v>
       </c>
       <c r="N13">
-        <v>-9999</v>
-      </c>
-      <c r="P13" s="5"/>
+        <v>22705.092540000001</v>
+      </c>
+      <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="C14">
-        <v>19546792</v>
+        <v>18565243</v>
       </c>
       <c r="D14">
-        <v>80.37</v>
-      </c>
-      <c r="E14">
-        <v>30687.754730000001</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>78.83</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="K14">
-        <v>59912431</v>
+        <v>58808266</v>
       </c>
       <c r="L14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M14">
-        <v>78.471000000000004</v>
+        <v>77.218000000000004</v>
       </c>
       <c r="N14">
-        <v>29478.999189999999</v>
+        <v>-9999</v>
       </c>
       <c r="P14" s="4"/>
     </row>
@@ -952,40 +933,77 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="C15">
-        <v>20434176</v>
+        <v>19546792</v>
       </c>
       <c r="D15">
-        <v>81.234999999999999</v>
+        <v>80.37</v>
       </c>
       <c r="E15">
-        <v>34435.367440000002</v>
-      </c>
-      <c r="G15" s="4"/>
+        <v>30687.754730000001</v>
+      </c>
+      <c r="G15" s="3"/>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="K15">
-        <v>60776238</v>
+        <v>59912431</v>
       </c>
       <c r="L15" t="s">
         <v>15</v>
       </c>
       <c r="M15">
+        <v>78.471000000000004</v>
+      </c>
+      <c r="N15">
+        <v>29478.999189999999</v>
+      </c>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2007</v>
+      </c>
+      <c r="C16">
+        <v>20434176</v>
+      </c>
+      <c r="D16">
+        <v>81.234999999999999</v>
+      </c>
+      <c r="E16">
+        <v>34435.367440000002</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16">
+        <v>2007</v>
+      </c>
+      <c r="K16">
+        <v>60776238</v>
+      </c>
+      <c r="L16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16">
         <v>79.424999999999997</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>33203.261279999999</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="6" t="s">
-        <v>18</v>
+    <row r="20" spans="1:1">
+      <c r="A20" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>